<commit_message>
update  user order service
</commit_message>
<xml_diff>
--- a/docs/设计文档/数据文档/数据结构.xlsx
+++ b/docs/设计文档/数据文档/数据结构.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24500" windowHeight="15620" tabRatio="690"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" r:id="rId1"/>
@@ -778,6 +778,166 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>主键ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brand_Cname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flag_Useable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car_Model_lv3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car_Outside_Color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car_Inside_Color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car_Addition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop_Stock</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Province_Cname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外观颜色集合，关联dic_color.id,逗号分割数组形式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电话</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮箱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店地址经度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外观颜色, Dic_Color.Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>内饰颜色，Dic_Color.Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车现货库存数量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User_City</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键城市,Dic_City.Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop_City</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Car_Sub_Brand</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车子品牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>db</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brand_Cname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nmber</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属品牌，外键：CarBrand.Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键Car_Sub_Brand.Id,可为空，为空说明无子品牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>SQL:
 --设置数据库级别字符集
 SET character_set_server = 'utf8';
@@ -791,168 +951,8 @@
        whaleuser IDENTIFIED BY 'whale'
     , whaleadmin IDENTIFIED BY 'whalefin403';
 --用户权限
-grant SELECT , DELETE , INSERT, UPDATE  ON TABLE whalecar.* to whaleuser;
+grant SELECT , DELETE , INSERT, UPDATE ,EXECUTE ON TABLE whalecar.* to whaleuser;
 grant ALL ON TABLE whalecar.* to whaleadmin;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>主键ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brand_Cname</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flag_Useable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car_Model_lv3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car_Outside_Color</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car_Inside_Color</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car_Addition</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop_Stock</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Province_Cname</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>外观颜色集合，关联dic_color.id,逗号分割数组形式</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>地址</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电话</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>邮箱</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商店地址经度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>外观颜色, Dic_Color.Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>内饰颜色，Dic_Color.Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>汽车现货库存数量</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>User_City</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键城市,Dic_City.Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shop_City</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Car_Sub_Brand</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>汽车子品牌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>db</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brand_Cname</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nmber</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>所属品牌，外键：CarBrand.Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>外键Car_Sub_Brand.Id,可为空，为空说明无子品牌</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1498,13 +1498,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
         <v>218</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>219</v>
-      </c>
-      <c r="C3" t="s">
-        <v>220</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="9" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1957,7 +1957,7 @@
         <v>159</v>
       </c>
       <c r="G6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2032,7 +2032,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
         <v>154</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
         <v>154</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
         <v>169</v>
@@ -2469,7 +2469,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>91</v>
@@ -2618,7 +2618,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -2635,21 +2635,21 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -2725,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2800,19 +2800,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" t="s">
         <v>223</v>
-      </c>
-      <c r="C4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3174,10 +3174,10 @@
         <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" t="s">
         <v>70</v>
@@ -3188,7 +3188,7 @@
         <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
         <v>77</v>
@@ -3208,7 +3208,7 @@
         <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3340,7 +3340,7 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s">
         <v>70</v>
@@ -3354,7 +3354,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
         <v>70</v>
@@ -3368,10 +3368,10 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3382,7 +3382,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
         <v>102</v>
@@ -3404,16 +3404,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" t="s">
         <v>214</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>215</v>
-      </c>
-      <c r="D9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3542,7 +3542,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
         <v>101</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
         <v>101</v>
@@ -3576,13 +3576,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
         <v>70</v>
@@ -3593,13 +3593,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
         <v>70</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>46</v>
@@ -3619,7 +3619,7 @@
         <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3644,7 +3644,7 @@
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9" t="s">
         <v>104</v>
@@ -3787,16 +3787,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
         <v>213</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>214</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>215</v>
-      </c>
-      <c r="D6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:7">

</xml_diff>